<commit_message>
Defined Unittests for LibraryItem, Made Client Program
</commit_message>
<xml_diff>
--- a/tests/test_plan_library_item.xlsx
+++ b/tests/test_plan_library_item.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Desktop\Intermediate Software Development0315\8. Activities\Module_01\given_files\activity_1\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\Documents\rrc-polytech\semester-2\intermediate_software_development\Activities\Activity-1\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94801D8B-F184-4C7C-AC17-1E2ABA18B123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CA83FA-1E7E-4BB1-AE0E-F71B441891C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -183,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -249,13 +247,73 @@
   </si>
   <si>
     <t>Attribute  set to input values.</t>
+  </si>
+  <si>
+    <t>Title is blank.</t>
+  </si>
+  <si>
+    <t>Author is blank.</t>
+  </si>
+  <si>
+    <t>Valid title, author, and genre values exist.</t>
+  </si>
+  <si>
+    <t>Genre is invalid.</t>
+  </si>
+  <si>
+    <t>LibraryItem object created with title set.</t>
+  </si>
+  <si>
+    <t>LibraryItem object created with author set.</t>
+  </si>
+  <si>
+    <t>LibraryItem object created with genre set.</t>
+  </si>
+  <si>
+    <t>"One Piece", "Eichiro Oda", Genre.FICTION</t>
+  </si>
+  <si>
+    <t>"", "Eichiro Oda", Genre.FICTION</t>
+  </si>
+  <si>
+    <t>"One Piece", "", Genre.FICTION</t>
+  </si>
+  <si>
+    <t>"One Piece", "Eichiro Oda", "Invalid"</t>
+  </si>
+  <si>
+    <t>Object created successfully with attributes set to input values.</t>
+  </si>
+  <si>
+    <t>Raises ValueError with message "Title cannot be blank."</t>
+  </si>
+  <si>
+    <t>Raises ValueError with message "Author cannot be blank."</t>
+  </si>
+  <si>
+    <t>Raises ValueError with message "Invalid Genre."</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Returns  "One Piece"</t>
+  </si>
+  <si>
+    <t>Returns 'Eichiro Oda'</t>
+  </si>
+  <si>
+    <t>Returns Genre.FICTION</t>
+  </si>
+  <si>
+    <t>Parth Joshi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -535,9 +593,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -552,6 +607,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1109,22 +1167,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" customWidth="1"/>
+    <col min="5" max="5" width="29.109375" customWidth="1"/>
+    <col min="6" max="6" width="35.44140625" customWidth="1"/>
+    <col min="7" max="7" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="1.45">
+    <row r="1" spans="1:7" ht="15" thickBot="1"/>
+    <row r="2" spans="1:7" ht="73.2" customHeight="1" thickBot="1">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -1136,26 +1194,28 @@
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15" thickBot="1">
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="16"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="15"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1">
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="18"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D4" s="17"/>
+    </row>
+    <row r="5" spans="1:7">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="B6" s="7" t="s">
         <v>0</v>
       </c>
@@ -1175,7 +1235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="78" customHeight="1">
       <c r="A7" s="4"/>
       <c r="B7" s="11">
         <v>1</v>
@@ -1186,11 +1246,17 @@
       <c r="D7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="66.75" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="12">
         <v>2</v>
@@ -1201,11 +1267,17 @@
       <c r="D8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="74.25" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="12">
         <v>3</v>
@@ -1216,11 +1288,17 @@
       <c r="D9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="78.75" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="11">
         <v>4</v>
@@ -1231,11 +1309,17 @@
       <c r="D10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="72" customHeight="1">
       <c r="B11" s="12">
         <v>5</v>
       </c>
@@ -1245,11 +1329,17 @@
       <c r="D11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="61.5" customHeight="1">
       <c r="B12" s="12">
         <v>6</v>
       </c>
@@ -1259,11 +1349,17 @@
       <c r="D12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="63.75" customHeight="1">
       <c r="B13" s="11">
         <v>7</v>
       </c>
@@ -1273,11 +1369,17 @@
       <c r="D13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="31.2" customHeight="1">
       <c r="B14" s="11">
         <v>10</v>
       </c>
@@ -1287,7 +1389,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="31.2" customHeight="1">
       <c r="B15" s="12">
         <v>11</v>
       </c>
@@ -1297,7 +1399,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="31.2" customHeight="1">
       <c r="B16" s="12">
         <v>12</v>
       </c>
@@ -1307,7 +1409,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" ht="31.2" customHeight="1">
       <c r="B17" s="11">
         <v>13</v>
       </c>
@@ -1317,7 +1419,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" ht="31.2" customHeight="1">
       <c r="B18" s="12">
         <v>14</v>
       </c>
@@ -1327,7 +1429,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="31.2" customHeight="1">
       <c r="B19" s="12">
         <v>15</v>
       </c>
@@ -1337,7 +1439,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" ht="31.2" customHeight="1">
       <c r="B20" s="11">
         <v>16</v>
       </c>
@@ -1347,7 +1449,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" ht="31.2" customHeight="1">
       <c r="B21" s="12">
         <v>17</v>
       </c>
@@ -1357,7 +1459,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="31.2" customHeight="1">
       <c r="B22" s="12">
         <v>18</v>
       </c>
@@ -1367,7 +1469,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" ht="31.2" customHeight="1">
       <c r="B23" s="11">
         <v>19</v>
       </c>
@@ -1377,7 +1479,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" ht="31.2" customHeight="1">
       <c r="B24" s="12">
         <v>20</v>
       </c>
@@ -1387,15 +1489,15 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="19" t="s">
+    <row r="26" spans="2:7">
+      <c r="B26" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1405,14 +1507,24 @@
     <mergeCell ref="B26:G26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003B3B6B51C940774DBF92367B1D1A75F0" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="80d4f13eaa95653e2ff902bb880fefc3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee0e594b-5dc6-49aa-9be8-f17bb89b127c" xmlns:ns3="b80edf0c-bd47-4bae-8c19-89fc2af9398f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ababe2f621e4b192c84b1cec6edec4f" ns2:_="" ns3:_="">
     <xsd:import namespace="ee0e594b-5dc6-49aa-9be8-f17bb89b127c"/>
@@ -1607,15 +1719,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1628,13 +1731,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37F01E9C-39D8-491B-950E-769C54FF39B2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3194B8C0-471E-4E12-8338-7B9268783B6C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3194B8C0-471E-4E12-8338-7B9268783B6C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37F01E9C-39D8-491B-950E-769C54FF39B2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ee0e594b-5dc6-49aa-9be8-f17bb89b127c"/>
+    <ds:schemaRef ds:uri="b80edf0c-bd47-4bae-8c19-89fc2af9398f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93494D4A-B25F-4AE9-9242-3524F3518EDF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93494D4A-B25F-4AE9-9242-3524F3518EDF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ee0e594b-5dc6-49aa-9be8-f17bb89b127c"/>
+    <ds:schemaRef ds:uri="b80edf0c-bd47-4bae-8c19-89fc2af9398f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Filled excel sheet and fixed minor issue in tests cases
</commit_message>
<xml_diff>
--- a/tests/test_plan_library_item.xlsx
+++ b/tests/test_plan_library_item.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\Documents\rrc-polytech\semester-2\intermediate_software_development\Activities\Activity-1\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CA83FA-1E7E-4BB1-AE0E-F71B441891C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4965021-0AD7-401A-B2E7-9A0C078FD094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -313,7 +313,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -593,6 +593,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -607,9 +610,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1167,22 +1167,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" customWidth="1"/>
-    <col min="5" max="5" width="29.109375" customWidth="1"/>
-    <col min="6" max="6" width="35.44140625" customWidth="1"/>
-    <col min="7" max="7" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1"/>
-    <row r="2" spans="1:7" ht="73.2" customHeight="1" thickBot="1">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="1.45">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -1194,28 +1194,28 @@
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="15"/>
-    </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1">
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="17"/>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="D4" s="18"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>0</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="78" customHeight="1">
+    <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="11">
         <v>1</v>
@@ -1256,7 +1256,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="66.75" customHeight="1">
+    <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="12">
         <v>2</v>
@@ -1277,7 +1277,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="74.25" customHeight="1">
+    <row r="9" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="12">
         <v>3</v>
@@ -1298,7 +1298,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="78.75" customHeight="1">
+    <row r="10" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="11">
         <v>4</v>
@@ -1319,7 +1319,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="72" customHeight="1">
+    <row r="11" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="12">
         <v>5</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="61.5" customHeight="1">
+    <row r="12" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="12">
         <v>6</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="63.75" customHeight="1">
+    <row r="13" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11">
         <v>7</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="31.2" customHeight="1">
+    <row r="14" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="11">
         <v>10</v>
       </c>
@@ -1389,7 +1389,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" ht="31.2" customHeight="1">
+    <row r="15" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="12">
         <v>11</v>
       </c>
@@ -1399,7 +1399,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="31.2" customHeight="1">
+    <row r="16" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="12">
         <v>12</v>
       </c>
@@ -1409,7 +1409,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="2:7" ht="31.2" customHeight="1">
+    <row r="17" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="11">
         <v>13</v>
       </c>
@@ -1419,7 +1419,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="2:7" ht="31.2" customHeight="1">
+    <row r="18" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12">
         <v>14</v>
       </c>
@@ -1429,7 +1429,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="2:7" ht="31.2" customHeight="1">
+    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="12">
         <v>15</v>
       </c>
@@ -1439,7 +1439,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="2:7" ht="31.2" customHeight="1">
+    <row r="20" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="11">
         <v>16</v>
       </c>
@@ -1449,7 +1449,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="2:7" ht="31.2" customHeight="1">
+    <row r="21" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="12">
         <v>17</v>
       </c>
@@ -1459,7 +1459,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="2:7" ht="31.2" customHeight="1">
+    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="12">
         <v>18</v>
       </c>
@@ -1469,7 +1469,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="2:7" ht="31.2" customHeight="1">
+    <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="11">
         <v>19</v>
       </c>
@@ -1479,7 +1479,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="2:7" ht="31.2" customHeight="1">
+    <row r="24" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="12">
         <v>20</v>
       </c>
@@ -1489,15 +1489,15 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="26" spans="2:7">
-      <c r="B26" s="18" t="s">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1516,12 +1516,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ee0e594b-5dc6-49aa-9be8-f17bb89b127c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b80edf0c-bd47-4bae-8c19-89fc2af9398f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1720,20 +1722,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ee0e594b-5dc6-49aa-9be8-f17bb89b127c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b80edf0c-bd47-4bae-8c19-89fc2af9398f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3194B8C0-471E-4E12-8338-7B9268783B6C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93494D4A-B25F-4AE9-9242-3524F3518EDF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ee0e594b-5dc6-49aa-9be8-f17bb89b127c"/>
+    <ds:schemaRef ds:uri="b80edf0c-bd47-4bae-8c19-89fc2af9398f"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1758,12 +1761,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93494D4A-B25F-4AE9-9242-3524F3518EDF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3194B8C0-471E-4E12-8338-7B9268783B6C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ee0e594b-5dc6-49aa-9be8-f17bb89b127c"/>
-    <ds:schemaRef ds:uri="b80edf0c-bd47-4bae-8c19-89fc2af9398f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Saved Excel test plan file
</commit_message>
<xml_diff>
--- a/tests/test_plan_library_item.xlsx
+++ b/tests/test_plan_library_item.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\Documents\rrc-polytech\semester-2\intermediate_software_development\Activities\Activity-1\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90DDF7B-3E78-4020-8D00-6D3599EA6306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1E685C-9F6C-48F7-B993-43CCD5372581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="-23148" yWindow="3900" windowWidth="23256" windowHeight="12456" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -297,9 +297,6 @@
     <t>Parth Joshi</t>
   </si>
   <si>
-    <t>1999,"One Piece", "Eichiro Oda", "Invalid"</t>
-  </si>
-  <si>
     <t>1999,"One Piece", "Eichiro Oda", Genre.FICTION,False</t>
   </si>
   <si>
@@ -349,6 +346,9 @@
   </si>
   <si>
     <t>Returns False</t>
+  </si>
+  <si>
+    <t>1999,"One Piece", "Eichiro Oda", "Invalid", False</t>
   </si>
 </sst>
 </file>
@@ -1209,8 +1209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1292,7 +1292,7 @@
         <v>24</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>29</v>
@@ -1313,7 +1313,7 @@
         <v>22</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>30</v>
@@ -1334,7 +1334,7 @@
         <v>23</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>31</v>
@@ -1355,7 +1355,7 @@
         <v>25</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>32</v>
@@ -1369,16 +1369,16 @@
         <v>8</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>33</v>
       </c>
       <c r="F11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="61.5" customHeight="1">
@@ -1389,16 +1389,16 @@
         <v>8</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>33</v>
       </c>
       <c r="F12" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="63.75" customHeight="1">
@@ -1466,19 +1466,19 @@
         <v>10</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="9" t="s">
         <v>49</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>50</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>33</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="31.15" customHeight="1">
@@ -1486,19 +1486,19 @@
         <v>11</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>54</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>33</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="31.15" customHeight="1">

</xml_diff>